<commit_message>
impl:导出补充 A4.五岁以下死亡监测 DeathMonitorUnder5Area B2.早产儿管理情况统计报 @夏锦慧 PrematureBabyManagementArea B3.医疗机构早产儿出生情况统计报表 YLJGZCECSQKTJJDBBArea B4.五岁以下死亡监测(季度报表) DeathMonitorUnder5QuarterlyArea
</commit_message>
<xml_diff>
--- a/VL.Research/XMLConfig/GWEArea/列表.xlsx
+++ b/VL.Research/XMLConfig/GWEArea/列表.xlsx
@@ -14,15 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>浙江省高危儿管</t>
     </r>
     <r>
@@ -30,7 +24,7 @@
         <b/>
         <sz val="18"/>
         <rFont val="Times New Roman"/>
-        <charset val="0"/>
+        <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -48,7 +42,7 @@
         <b/>
         <sz val="18"/>
         <rFont val="Times New Roman"/>
-        <charset val="0"/>
+        <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -66,7 +60,7 @@
         <b/>
         <sz val="18"/>
         <rFont val="Times New Roman"/>
-        <charset val="0"/>
+        <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -84,7 +78,7 @@
         <b/>
         <sz val="18"/>
         <rFont val="Times New Roman"/>
-        <charset val="0"/>
+        <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -102,7 +96,7 @@
         <b/>
         <sz val="18"/>
         <rFont val="Times New Roman"/>
-        <charset val="0"/>
+        <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -113,7 +107,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>表（1季度）</t>
+      <t>表</t>
     </r>
   </si>
   <si>
@@ -189,18 +183,6 @@
       </rPr>
       <t>％</t>
     </r>
-  </si>
-  <si>
-    <t>PN分类求和</t>
-  </si>
-  <si>
-    <t>shenhuatable</t>
-  </si>
-  <si>
-    <t>hcgSumInt</t>
-  </si>
-  <si>
-    <t>hcgSumCase</t>
   </si>
   <si>
     <t>早产儿</t>
@@ -343,9 +325,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
@@ -403,9 +385,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -419,6 +407,50 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
@@ -426,16 +458,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -457,74 +513,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -533,15 +521,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -550,7 +532,7 @@
       <b/>
       <sz val="18"/>
       <name val="Times New Roman"/>
-      <charset val="0"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
@@ -573,43 +555,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,7 +579,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -639,13 +609,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -657,7 +627,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,7 +657,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,7 +687,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,25 +699,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -723,25 +711,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -867,6 +849,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -878,30 +878,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -923,15 +899,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -941,11 +908,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -970,10 +952,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -982,133 +964,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1514,7 +1496,7 @@
   <dimension ref="A1:XEM16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A1" sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28333333333333" defaultRowHeight="13.5"/>
@@ -17956,7 +17938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="15" spans="1:20">
+    <row r="4" s="1" customFormat="1" ht="15" spans="1:17">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="9" t="s">
@@ -17991,39 +17973,28 @@
         <v>17</v>
       </c>
       <c r="P4" s="9"/>
-      <c r="Q4" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="Q4" s="28"/>
     </row>
-    <row r="5" customFormat="1" ht="14.25" spans="1:20">
+    <row r="5" customFormat="1" ht="14.25" spans="1:16">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -18033,126 +18004,110 @@
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
-      <c r="Q5" t="str">
-        <f>"@Loop1000_Data_"&amp;Q4</f>
-        <v>@Loop1000_Data_PN分类求和</v>
-      </c>
-      <c r="R5" t="str">
-        <f>"@Loop1000_Data_"&amp;R4</f>
-        <v>@Loop1000_Data_shenhuatable</v>
-      </c>
-      <c r="S5" t="str">
-        <f>"@Loop1000_Data_"&amp;S4</f>
-        <v>@Loop1000_Data_hcgSumInt</v>
-      </c>
-      <c r="T5" t="str">
-        <f>"@Loop1000_Data_"&amp;T4</f>
-        <v>@Loop1000_Data_hcgSumCase</v>
-      </c>
     </row>
     <row r="6" ht="14.25" spans="1:16">
       <c r="A6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="J6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="L6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="M6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="N6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="O6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="P6" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" ht="14.25" spans="1:16">
       <c r="A7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="I7" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="J7" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="K7" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="L7" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="M7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="N7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="O7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="L7" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>57</v>
-      </c>
       <c r="P7" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" ht="14.25" spans="1:16">
       <c r="A8" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -18172,7 +18127,7 @@
     </row>
     <row r="9" ht="14.25" spans="1:16">
       <c r="A9" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -18192,7 +18147,7 @@
     </row>
     <row r="10" ht="14.25" spans="1:16">
       <c r="A10" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -18212,7 +18167,7 @@
     </row>
     <row r="11" ht="14.25" spans="1:16">
       <c r="A11" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -18253,7 +18208,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -18275,7 +18230,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="20"/>
@@ -18294,10 +18249,10 @@
     </row>
     <row r="15" ht="14.25" spans="1:16">
       <c r="A15" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -18319,7 +18274,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>

</xml_diff>